<commit_message>
change to variety score
</commit_message>
<xml_diff>
--- a/plot/other/tradeoff.xlsx
+++ b/plot/other/tradeoff.xlsx
@@ -1,35 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuboluo/Documents/PycharmProjects/SmartSwitch/plot/other/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB4536E-420C-434E-8715-3708928D4DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Score</t>
+    <t>Budget</t>
   </si>
   <si>
-    <t>Overhead</t>
+    <t>Similarity Score</t>
   </si>
   <si>
-    <t>Budget</t>
+    <t>Overhead Reduction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +72,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -112,7 +126,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -144,9 +158,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,6 +210,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,25 +403,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -382,9 +438,9 @@
         <v>98374</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>0.06068268341755383</v>
+        <v>6.0682683417553833E-2</v>
       </c>
       <c r="B3">
         <v>0.9488047387349271</v>
@@ -393,97 +449,97 @@
         <v>104182</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>0.3135275647813963</v>
+        <v>0.31352756478139632</v>
       </c>
       <c r="B4">
-        <v>0.7263944714759185</v>
+        <v>0.72639447147591851</v>
       </c>
       <c r="C4">
         <v>135622</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>0.4029810662083615</v>
+        <v>0.40298106620836149</v>
       </c>
       <c r="B5">
-        <v>0.6751992102108456</v>
+        <v>0.67519921021084561</v>
       </c>
       <c r="C5">
         <v>141430</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>0.4165905908821862</v>
       </c>
       <c r="B6">
-        <v>0.6325364924899514</v>
+        <v>0.63253649248995136</v>
       </c>
       <c r="C6">
         <v>147238</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>0.5082158334557345</v>
+        <v>0.50821583345573451</v>
       </c>
       <c r="B7">
-        <v>0.5075100486566533</v>
+        <v>0.50751004865665328</v>
       </c>
       <c r="C7">
         <v>172870</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>0.5976693348826991</v>
+        <v>0.59766933488269913</v>
       </c>
       <c r="B8">
-        <v>0.4563147873915803</v>
+        <v>0.45631478739158032</v>
       </c>
       <c r="C8">
         <v>178678</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>0.6112788595565238</v>
+        <v>0.61127885955652383</v>
       </c>
       <c r="B9">
-        <v>0.4136520696706861</v>
+        <v>0.41365206967068607</v>
       </c>
       <c r="C9">
         <v>184486</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>0.6157495802107392</v>
+        <v>0.61574958021073922</v>
       </c>
       <c r="B10">
-        <v>0.3795218954939709</v>
+        <v>0.37952189549397092</v>
       </c>
       <c r="C10">
         <v>190294</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>0.6330303091531022</v>
+        <v>0.63303030915310221</v>
       </c>
       <c r="B11">
-        <v>0.3433467315422044</v>
+        <v>0.34334673154220441</v>
       </c>
       <c r="C11">
         <v>210118</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>0.6937129925706561</v>
+        <v>0.69371299257065611</v>
       </c>
       <c r="B12">
         <v>0.2921514702771314</v>
@@ -492,9 +548,9 @@
         <v>215926</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>0.7177509694617618</v>
+        <v>0.71775096946176176</v>
       </c>
       <c r="B13">
         <v>0.2494887525562372</v>
@@ -503,20 +559,20 @@
         <v>221734</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>0.7268072815640092</v>
       </c>
       <c r="B14">
-        <v>0.2153585783795219</v>
+        <v>0.21535857837952191</v>
       </c>
       <c r="C14">
         <v>227542</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>0.7322410688253579</v>
+        <v>0.73224106882535789</v>
       </c>
       <c r="B15">
         <v>0.1897609477469854</v>
@@ -525,9 +581,9 @@
         <v>233350</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>0.7322410688253579</v>
+        <v>0.73224106882535789</v>
       </c>
       <c r="B16">
         <v>0.1897609477469854</v>
@@ -536,9 +592,9 @@
         <v>247366</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>0.768975017472726</v>
+        <v>0.76897501747272601</v>
       </c>
       <c r="B17">
         <v>0.1315139976024258</v>
@@ -547,117 +603,117 @@
         <v>253174</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>0.7920206495537543</v>
+        <v>0.79202064955375429</v>
       </c>
       <c r="B18">
-        <v>0.1144489105140681</v>
+        <v>0.11444891051406809</v>
       </c>
       <c r="C18">
         <v>258982</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>0.8096626109852246</v>
+        <v>0.80966261098522463</v>
       </c>
       <c r="B19">
-        <v>0.1059163669698893</v>
+        <v>0.10591636696988931</v>
       </c>
       <c r="C19">
         <v>264790</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>0.8161675678805578</v>
+        <v>0.81616756788055778</v>
       </c>
       <c r="B20">
-        <v>0.0803187363373528</v>
+        <v>8.03187363373528E-2</v>
       </c>
       <c r="C20">
         <v>270598</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>0.8181806228942555</v>
+        <v>0.81818062289425553</v>
       </c>
       <c r="B21">
-        <v>0.06325364924899514</v>
+        <v>6.3253649248995139E-2</v>
       </c>
       <c r="C21">
         <v>276406</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>0.8790540912823496</v>
+        <v>0.87905409128234957</v>
       </c>
       <c r="B22">
-        <v>0.06325364924899514</v>
+        <v>6.3253649248995139E-2</v>
       </c>
       <c r="C22">
         <v>284614</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>0.9685075927093147</v>
+        <v>0.96850759270931475</v>
       </c>
       <c r="B23">
-        <v>0.06325364924899514</v>
+        <v>6.3253649248995139E-2</v>
       </c>
       <c r="C23">
         <v>290422</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>0.9822349288282973</v>
+        <v>0.98223492882829733</v>
       </c>
       <c r="B24">
-        <v>0.06325364924899514</v>
+        <v>6.3253649248995139E-2</v>
       </c>
       <c r="C24">
         <v>296230</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>0.9885968102902494</v>
+        <v>0.98859681029024937</v>
       </c>
       <c r="B25">
-        <v>0.05119526126507299</v>
+        <v>5.119526126507299E-2</v>
       </c>
       <c r="C25">
         <v>302038</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>0.9928155499340123</v>
+        <v>0.99281554993401233</v>
       </c>
       <c r="B26">
-        <v>0.0255976306325365</v>
+        <v>2.5597630632536499E-2</v>
       </c>
       <c r="C26">
         <v>307846</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>0.9967273294863562</v>
+        <v>0.99672732948635623</v>
       </c>
       <c r="B27">
-        <v>0.008532543544178832</v>
+        <v>8.5325435441788323E-3</v>
       </c>
       <c r="C27">
         <v>313654</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>

</xml_diff>